<commit_message>
fixed lr at 0.5 for base
</commit_message>
<xml_diff>
--- a/rn_holdout.xlsx
+++ b/rn_holdout.xlsx
@@ -395,12 +395,12 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.90625" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="5" min="5" style="3" width="14.85546875"/>
+    <col customWidth="1" max="5" min="5" style="3" width="14.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -440,13 +440,13 @@
         <v>60</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0005</v>
+        <v>0.5</v>
       </c>
       <c r="F2" t="n">
-        <v>0.420625</v>
+        <v>0.7678125</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5921689397272327</v>
+        <v>0.7688129035678574</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -463,13 +463,13 @@
         <v>60</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0005</v>
+        <v>0.5</v>
       </c>
       <c r="F3" t="n">
-        <v>0.420625</v>
+        <v>0.776875</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5921689397272327</v>
+        <v>0.7781903995587898</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -486,13 +486,13 @@
         <v>60</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0005</v>
+        <v>0.5</v>
       </c>
       <c r="F4" t="n">
-        <v>0.420625</v>
+        <v>0.778125</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5921689397272327</v>
+        <v>0.7794271079322289</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -509,13 +509,13 @@
         <v>60</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0005</v>
+        <v>0.5</v>
       </c>
       <c r="F5" t="n">
-        <v>0.420625</v>
+        <v>0.579375</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5921689397272327</v>
+        <v>0.7336762960031658</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -532,13 +532,13 @@
         <v>30</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0005</v>
+        <v>0.5</v>
       </c>
       <c r="F6" t="n">
-        <v>0.420625</v>
+        <v>0.7603124999999999</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5921689397272327</v>
+        <v>0.7611860454996487</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -555,13 +555,13 @@
         <v>120</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0005</v>
+        <v>0.5</v>
       </c>
       <c r="F7" t="n">
-        <v>0.420625</v>
+        <v>0.7884375</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5921689397272327</v>
+        <v>0.7897762549501113</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -578,13 +578,13 @@
         <v>240</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0005</v>
+        <v>0.5</v>
       </c>
       <c r="F8" t="n">
-        <v>0.420625</v>
+        <v>0.7865625000000001</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5921689397272327</v>
+        <v>0.7877376837176459</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -601,7 +601,7 @@
         <v>60</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0005</v>
+        <v>0.5</v>
       </c>
       <c r="F9" t="n">
         <v>0.420625</v>
@@ -624,7 +624,7 @@
         <v>60</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0005</v>
+        <v>0.5</v>
       </c>
       <c r="F10" t="n">
         <v>0.420625</v>
@@ -647,7 +647,7 @@
         <v>60</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0005</v>
+        <v>0.5</v>
       </c>
       <c r="F11" t="n">
         <v>0.420625</v>
@@ -673,10 +673,10 @@
         <v>0.1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7378125</v>
+        <v>0.720625</v>
       </c>
       <c r="G12" t="n">
-        <v>0.7394442836433029</v>
+        <v>0.70841279346272</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -696,10 +696,10 @@
         <v>0.5</v>
       </c>
       <c r="F13" t="n">
-        <v>0.78125</v>
+        <v>0.7940625</v>
       </c>
       <c r="G13" t="n">
-        <v>0.7826182872695882</v>
+        <v>0.7945738143674341</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -719,10 +719,10 @@
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>0.785625</v>
+        <v>0.7925</v>
       </c>
       <c r="G14" t="n">
-        <v>0.7868859915871931</v>
+        <v>0.7936019512183544</v>
       </c>
     </row>
     <row r="15" spans="1:7">

</xml_diff>